<commit_message>
Contact us tab added, date format changed, searchable car database restricted to cars younger than 10 years
</commit_message>
<xml_diff>
--- a/Laszlo_Papp/Training/Motor/PackageGridCalculationExcel.xlsx
+++ b/Laszlo_Papp/Training/Motor/PackageGridCalculationExcel.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Documents\Git Repos\Training sandbox\Laszlo_Papp\Training\Motor\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5ED89D37-ADF2-4364-9755-B8654946E23F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A6D69BAB-2DE3-494C-A71F-D46B34C1B806}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="915" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="30" windowWidth="29040" windowHeight="15840" tabRatio="915" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Skye Lookup Input" sheetId="41" r:id="rId1"/>
@@ -120,7 +120,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="18">
   <si>
     <t>Skye Attribute Value</t>
   </si>
@@ -167,22 +167,13 @@
     <t>Skye attribute Value#10</t>
   </si>
   <si>
-    <t>Packages.BasicPackage</t>
-  </si>
-  <si>
-    <t>Packages.PremiumLightPackage</t>
-  </si>
-  <si>
-    <t>Packages.PremiumPlusPackage</t>
-  </si>
-  <si>
-    <t>Basic Package</t>
-  </si>
-  <si>
-    <t>Premium Light Package</t>
-  </si>
-  <si>
-    <t>Premium Plus Package</t>
+    <t>PackagePrice</t>
+  </si>
+  <si>
+    <t>GridPackageSelection.PackagePrice</t>
+  </si>
+  <si>
+    <t>GridPackageSelection.PackagesGridColoumn</t>
   </si>
 </sst>
 </file>
@@ -627,7 +618,7 @@
   <dimension ref="A1:IV5"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -925,7 +916,7 @@
     </row>
     <row r="2" spans="1:256" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B2" s="2" t="b">
         <v>0</v>
@@ -936,23 +927,12 @@
     </row>
     <row r="3" spans="1:256" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B3" s="2" t="b">
         <v>0</v>
       </c>
       <c r="C3" s="2" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4" spans="1:256" x14ac:dyDescent="0.3">
-      <c r="A4" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="B4" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="C4" s="2" t="b">
         <v>1</v>
       </c>
     </row>
@@ -1032,10 +1012,10 @@
   <sheetPr>
     <tabColor theme="2" tint="-0.749992370372631"/>
   </sheetPr>
-  <dimension ref="A1:B4"/>
+  <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1054,29 +1034,11 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="B2" s="2" t="str">
-        <f>IF('Skye Lookup Input'!D2&lt;&gt;"",'Skye Lookup Input'!D2,"")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A3" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="B3" s="2" t="str">
-        <f>IF('Skye Lookup Input'!D3&lt;&gt;"",'Skye Lookup Input'!D3,"")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A4" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="B4" s="2" t="str">
-        <f>IF('Skye Lookup Input'!D4&lt;&gt;"",'Skye Lookup Input'!D4,"")</f>
-        <v/>
+        <v>15</v>
+      </c>
+      <c r="B2" s="2">
+        <f>'Skye Lookup Input'!D3</f>
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>